<commit_message>
PLS 1month with new parameters
</commit_message>
<xml_diff>
--- a/4.MultivariteDataAnalysis/ModelCoefficients.xlsx
+++ b/4.MultivariteDataAnalysis/ModelCoefficients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isak.skeie\Documents\MasterAdventure\4.MultivariteDataAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\MasterAdventure\4.MultivariteDataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40F9FF9-AAE3-4964-A7C9-D3F90F634DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A4EE28-2BB3-44C4-8582-A537869634EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Model</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>0.47</t>
+  </si>
+  <si>
+    <t>0.4315</t>
+  </si>
+  <si>
+    <t>0.3538</t>
+  </si>
+  <si>
+    <t>0.2779</t>
+  </si>
+  <si>
+    <t>PLS</t>
+  </si>
+  <si>
+    <t>PLS on data with 1h sampling over 1 month</t>
   </si>
 </sst>
 </file>
@@ -419,26 +434,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -506,6 +521,41 @@
       </c>
       <c r="K2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>-0.4345</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <v>-0.1648</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <v>-0.13689999999999999</v>
+      </c>
+      <c r="J3">
+        <v>-0.1842</v>
+      </c>
+      <c r="K3">
+        <v>0.58599999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change in prediction CSV file
</commit_message>
<xml_diff>
--- a/4.MultivariteDataAnalysis/ModelCoefficients.xlsx
+++ b/4.MultivariteDataAnalysis/ModelCoefficients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isak.skeie\Documents\MasterAdventure\4.MultivariteDataAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\MasterAdventure\4.MultivariteDataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AEA13A-1AE6-4A46-880A-C5B973D7F82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E923279F-BD22-468F-A12B-6D8F0197027A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="23010" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Model</t>
   </si>
@@ -154,6 +154,36 @@
   </si>
   <si>
     <t>0.586</t>
+  </si>
+  <si>
+    <t>PLS_predict</t>
+  </si>
+  <si>
+    <t>PLS with pediction on 1h into the future</t>
+  </si>
+  <si>
+    <t>0.427</t>
+  </si>
+  <si>
+    <t>-0.469</t>
+  </si>
+  <si>
+    <t>0.251</t>
+  </si>
+  <si>
+    <t>-0.179</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>-0.173</t>
+  </si>
+  <si>
+    <t>-0.205</t>
+  </si>
+  <si>
+    <t>0.588</t>
   </si>
 </sst>
 </file>
@@ -482,26 +512,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -571,7 +601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -606,7 +636,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -639,6 +669,41 @@
       </c>
       <c r="K4" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2 models to python
</commit_message>
<xml_diff>
--- a/4.MultivariteDataAnalysis/ModelCoefficients.xlsx
+++ b/4.MultivariteDataAnalysis/ModelCoefficients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\MasterAdventure\4.MultivariteDataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E923279F-BD22-468F-A12B-6D8F0197027A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770982FF-A735-452A-BCF9-2ABBD8C0B92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Model</t>
   </si>
@@ -162,28 +162,61 @@
     <t>PLS with pediction on 1h into the future</t>
   </si>
   <si>
-    <t>0.427</t>
-  </si>
-  <si>
-    <t>-0.469</t>
-  </si>
-  <si>
-    <t>0.251</t>
-  </si>
-  <si>
-    <t>-0.179</t>
-  </si>
-  <si>
-    <t>0.29</t>
-  </si>
-  <si>
-    <t>-0.173</t>
-  </si>
-  <si>
-    <t>-0.205</t>
-  </si>
-  <si>
-    <t>0.588</t>
+    <t>0.428</t>
+  </si>
+  <si>
+    <t>-0.433</t>
+  </si>
+  <si>
+    <t>0.367</t>
+  </si>
+  <si>
+    <t>-0.143</t>
+  </si>
+  <si>
+    <t>0.27</t>
+  </si>
+  <si>
+    <t>-0.128</t>
+  </si>
+  <si>
+    <t>-0.181</t>
+  </si>
+  <si>
+    <t>0.593</t>
+  </si>
+  <si>
+    <t>PLS LOG</t>
+  </si>
+  <si>
+    <t>PLS with log of turb</t>
+  </si>
+  <si>
+    <t>0.389</t>
+  </si>
+  <si>
+    <t>-0.446</t>
+  </si>
+  <si>
+    <t>-0.259</t>
+  </si>
+  <si>
+    <t>0.300</t>
+  </si>
+  <si>
+    <t>-0.110</t>
+  </si>
+  <si>
+    <t>0.256</t>
+  </si>
+  <si>
+    <t>-0.176</t>
+  </si>
+  <si>
+    <t>-0.243</t>
+  </si>
+  <si>
+    <t>0.570</t>
   </si>
 </sst>
 </file>
@@ -512,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,6 +739,41 @@
         <v>52</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>